<commit_message>
feat: :lipstick: EXCEL AL 90%
</commit_message>
<xml_diff>
--- a/storage/app/public/Templates/Excel/template_conteo.xlsx
+++ b/storage/app/public/Templates/Excel/template_conteo.xlsx
@@ -20,27 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
-  <si>
-    <t xml:space="preserve">CONTEO DE EXAMENES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xddx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t xml:space="preserve">UNIDAD DE RED DE LABORATORIOS -OADyLSP-DMyGS-DIRIS L.S.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INFORME ESTADISTICO DE LA PRODUCCIÓN DE ACTIVIDADES Y ANALISIS CLINICOS DE LABORATORIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N.º</t>
   </si>
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
   <si>
     <t xml:space="preserve">Cantidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:)</t>
   </si>
 </sst>
 </file>
@@ -50,7 +44,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -71,6 +65,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -129,16 +130,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -154,100 +179,110 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>332280</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>214920</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>111240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Imagen 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:srcRect l="0" t="73284" r="14016" b="0"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1147680" y="0"/>
+          <a:ext cx="4097880" cy="599040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A5:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.48"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F2" s="0" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="0" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F4" s="0" t="s">
+      <c r="B9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J5" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J6" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J7" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J9" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J12" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J13" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="0" t="s">
-        <v>2</v>
-      </c>
+      <c r="D9" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -255,5 +290,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>